<commit_message>
Insert Multiple records into different object using SOAP
</commit_message>
<xml_diff>
--- a/me/2.SOAP-API.xlsx
+++ b/me/2.SOAP-API.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce-integration-with-external-systems\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEA3B12-8462-4C02-9959-DBBF1822FE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7CED29-7BA9-4C98-A490-8C6D9D46E21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Authenticating SOAP API Users" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="SOAPQueryStudent" sheetId="3" r:id="rId3"/>
     <sheet name="InsertNewStudentWithMru" sheetId="4" r:id="rId4"/>
     <sheet name="InsertMultiplSchoolRecords" sheetId="5" r:id="rId5"/>
+    <sheet name="InsertMultipleRecordTypes" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="196">
   <si>
     <t>https://www.postman.com/salesforce-developers/workspace/salesforce-developers/request/</t>
   </si>
@@ -839,6 +840,82 @@
   </si>
   <si>
     <t>Object được tạo ra có thể xem được ở  "Recently Viewed"</t>
+  </si>
+  <si>
+    <t>Insert Multiple records into different object using SOAP</t>
+  </si>
+  <si>
+    <t>6.InsertMultipleRecordTypes.txt</t>
+  </si>
+  <si>
+    <t>salesforce-integration-with-external-systems\2.SOAP-API\6.InsertMultipleRecordTypes.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;urn:updateMru&gt;true&lt;/urn:updateMru&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           &lt;Name&gt;Blooming Dales International School&lt;/Name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           &lt;School_Address__c&gt;South Carolina&lt;/School_Address__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           &lt;School_Phone__c&gt;1110985555&lt;/School_Phone__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;Student_Name__c&gt;Sunny Malhotra&lt;/Student_Name__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;Phone_Number__c&gt;7890987777&lt;/Phone_Number__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;Email__c&gt;sunny_mal@hotmail.com&lt;/Email__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;Student_Name__c&gt;Neha Sidana&lt;/Student_Name__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;Phone_Number__c&gt;6780987777&lt;/Phone_Number__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;Email__c&gt;nehaSd@gmail.com&lt;/Email__c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;School__c&gt;a0B5g00000tpvm9EAA&lt;/School__c&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         &lt;urn:sObjects xsi:type="urn1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Student__c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Tạo 1 object school và 2 object Student</t>
+  </si>
+  <si>
+    <t>Một School mới được tạo</t>
+  </si>
+  <si>
+    <t>2 Student mới được tạo</t>
   </si>
 </sst>
 </file>
@@ -3378,6 +3455,643 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A913229-EA15-E0F3-0DB8-38A9E5EB69B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="3590925"/>
+          <a:ext cx="1819275" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCCA70C0-CEC2-D7E3-DF3D-48F6FFCD687B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885950" y="3571875"/>
+          <a:ext cx="1047750" cy="4133850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB5F724-3D48-2137-C773-CA704585972D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885950" y="3581400"/>
+          <a:ext cx="866775" cy="5238750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>286365</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171187</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{681C7CEC-C178-38C8-CB40-3E307D094D4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11575676" y="3686735"/>
+          <a:ext cx="12915395" cy="6580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>437030</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8DDEA62-8921-8D5E-9659-7070AE955BF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3025588" y="3978088"/>
+          <a:ext cx="14354736" cy="4471147"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>549088</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB4CA821-8343-4A33-E38B-91C9F1EF5543}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2969559" y="4011706"/>
+          <a:ext cx="14433176" cy="5602941"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>123266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>398582</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>168090</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC9D8BA-221A-E749-D797-16DF345A54DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739588" y="10791266"/>
+          <a:ext cx="11156229" cy="6331324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>431926</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCEF02EF-8418-0B2A-EC4E-DECEEBB5BA08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="750795" y="17268265"/>
+          <a:ext cx="11178366" cy="4885764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>168089</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>212913</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>78679</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA20D721-F63C-DB3B-8FDE-444C55694BD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="773207" y="22792764"/>
+          <a:ext cx="10936941" cy="3955915"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>537883</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56BAD0B8-693F-0028-AC7E-6D2FDC86484E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1748118" y="13155706"/>
+          <a:ext cx="739588" cy="12158382"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156881</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>201705</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>118048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8EFD6DC-032A-B093-DE71-D805F8818E73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="761999" y="27499236"/>
+          <a:ext cx="10936941" cy="4051312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>70890</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10BDE199-D06D-2CDB-49EB-88855615B640}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="31712648"/>
+          <a:ext cx="11060206" cy="5505742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>168088</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>79130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BB628AA-5F62-1D9F-2E5A-CA495A0FEFF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="773206" y="37450059"/>
+          <a:ext cx="10903323" cy="5491571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8837,8 +9551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA659F0-7DFB-40C2-9DCA-7DEA63F8C733}">
   <dimension ref="A4:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8889,14 +9603,14 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" t="s">
         <v>132</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" t="s">
         <v>133</v>
       </c>
       <c r="H11" s="9"/>
@@ -8958,47 +9672,375 @@
       <c r="B19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
       <c r="R19" s="9"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
       <c r="R20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>137</v>
+      </c>
+      <c r="R21" s="9"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="R22" s="9"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="R23" s="9"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R24" s="9"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="R25" s="9"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="R27" s="9"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="R28" s="9"/>
+      <c r="S28" t="s">
+        <v>25</v>
+      </c>
+      <c r="T28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="R29" s="9"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R30" s="9"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R31" s="9"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="R32" s="9"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="R33" s="9"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="R34" s="9"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="R35" s="9"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="R36" s="9"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="R37" s="9"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="R38" s="9"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="R39" s="9"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="R40" s="9"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="R41" s="9"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="R42" s="9"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="R43" s="9"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="R44" s="9"/>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="R45" s="9"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="R46" s="9"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="R47" s="9"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="R48" s="9"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="R49" s="9"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="R50" s="9"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="R51" s="9"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="R52" s="9"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B53" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB65C6AE-6AD1-4980-B1D0-74AC277A4B34}">
+  <dimension ref="A2:T226"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V143" sqref="V143"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="D12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="D13" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="D14" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -9017,9 +10059,9 @@
       <c r="Q21" s="17"/>
       <c r="R21" s="9"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -9038,9 +10080,9 @@
       <c r="Q22" s="17"/>
       <c r="R22" s="9"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -9059,9 +10101,9 @@
       <c r="Q23" s="17"/>
       <c r="R23" s="9"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>42</v>
+        <v>138</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -9080,9 +10122,9 @@
       <c r="Q24" s="17"/>
       <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -9101,9 +10143,9 @@
       <c r="Q25" s="17"/>
       <c r="R25" s="9"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -9122,9 +10164,9 @@
       <c r="Q26" s="17"/>
       <c r="R26" s="9"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -9143,9 +10185,9 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="9"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>159</v>
+        <v>43</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -9163,16 +10205,10 @@
       <c r="P28" s="17"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="9"/>
-      <c r="S28" t="s">
-        <v>25</v>
-      </c>
-      <c r="T28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -9191,9 +10227,9 @@
       <c r="Q29" s="17"/>
       <c r="R29" s="9"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -9212,9 +10248,9 @@
       <c r="Q30" s="17"/>
       <c r="R30" s="9"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -9233,9 +10269,9 @@
       <c r="Q31" s="17"/>
       <c r="R31" s="9"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>141</v>
+        <v>44</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -9256,7 +10292,7 @@
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -9277,7 +10313,7 @@
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -9298,7 +10334,7 @@
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -9319,7 +10355,7 @@
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -9340,7 +10376,7 @@
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -9361,7 +10397,7 @@
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
@@ -9382,7 +10418,7 @@
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -9403,7 +10439,7 @@
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -9424,7 +10460,7 @@
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -9445,7 +10481,7 @@
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -9466,7 +10502,7 @@
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -9487,7 +10523,7 @@
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
@@ -9508,7 +10544,7 @@
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
@@ -9529,7 +10565,7 @@
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -9550,7 +10586,7 @@
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -9571,7 +10607,7 @@
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -9592,7 +10628,7 @@
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -9613,7 +10649,7 @@
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
@@ -9634,7 +10670,7 @@
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
@@ -9655,7 +10691,7 @@
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
@@ -9675,25 +10711,2297 @@
       <c r="R52" s="9"/>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="9"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17"/>
+      <c r="R54" s="9"/>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B55" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="6"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="6"/>
+    </row>
+    <row r="119" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+      <c r="L119" s="2"/>
+      <c r="M119" s="2"/>
+      <c r="N119" s="2"/>
+      <c r="O119" s="2"/>
+      <c r="P119" s="2"/>
+      <c r="Q119" s="2"/>
+      <c r="R119" s="2"/>
+      <c r="S119" s="2"/>
+      <c r="T119" s="3"/>
+    </row>
+    <row r="120" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B120" s="8"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17"/>
+      <c r="I120" s="17"/>
+      <c r="J120" s="17"/>
+      <c r="K120" s="17"/>
+      <c r="L120" s="17"/>
+      <c r="M120" s="17"/>
+      <c r="N120" s="17"/>
+      <c r="O120" s="17"/>
+      <c r="P120" s="17"/>
+      <c r="Q120" s="17"/>
+      <c r="R120" s="17"/>
+      <c r="S120" s="17"/>
+      <c r="T120" s="9"/>
+    </row>
+    <row r="121" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B121" s="8"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="17"/>
+      <c r="J121" s="17"/>
+      <c r="K121" s="17"/>
+      <c r="L121" s="17"/>
+      <c r="M121" s="17"/>
+      <c r="N121" s="17"/>
+      <c r="O121" s="17"/>
+      <c r="P121" s="17"/>
+      <c r="Q121" s="17"/>
+      <c r="R121" s="17"/>
+      <c r="S121" s="17"/>
+      <c r="T121" s="9"/>
+    </row>
+    <row r="122" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B122" s="8"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="17"/>
+      <c r="H122" s="17"/>
+      <c r="I122" s="17"/>
+      <c r="J122" s="17"/>
+      <c r="K122" s="17"/>
+      <c r="L122" s="17"/>
+      <c r="M122" s="17"/>
+      <c r="N122" s="17"/>
+      <c r="O122" s="17"/>
+      <c r="P122" s="17"/>
+      <c r="Q122" s="17"/>
+      <c r="R122" s="17"/>
+      <c r="S122" s="17"/>
+      <c r="T122" s="9"/>
+    </row>
+    <row r="123" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B123" s="8"/>
+      <c r="C123" s="17"/>
+      <c r="D123" s="17"/>
+      <c r="E123" s="17"/>
+      <c r="F123" s="17"/>
+      <c r="G123" s="17"/>
+      <c r="H123" s="17"/>
+      <c r="I123" s="17"/>
+      <c r="J123" s="17"/>
+      <c r="K123" s="17"/>
+      <c r="L123" s="17"/>
+      <c r="M123" s="17"/>
+      <c r="N123" s="17"/>
+      <c r="O123" s="17"/>
+      <c r="P123" s="17"/>
+      <c r="Q123" s="17"/>
+      <c r="R123" s="17"/>
+      <c r="S123" s="17"/>
+      <c r="T123" s="9"/>
+    </row>
+    <row r="124" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B124" s="8"/>
+      <c r="C124" s="17"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="17"/>
+      <c r="F124" s="17"/>
+      <c r="G124" s="17"/>
+      <c r="H124" s="17"/>
+      <c r="I124" s="17"/>
+      <c r="J124" s="17"/>
+      <c r="K124" s="17"/>
+      <c r="L124" s="17"/>
+      <c r="M124" s="17"/>
+      <c r="N124" s="17"/>
+      <c r="O124" s="17"/>
+      <c r="P124" s="17"/>
+      <c r="Q124" s="17"/>
+      <c r="R124" s="17"/>
+      <c r="S124" s="17"/>
+      <c r="T124" s="9"/>
+    </row>
+    <row r="125" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B125" s="8"/>
+      <c r="C125" s="17"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="17"/>
+      <c r="F125" s="17"/>
+      <c r="G125" s="17"/>
+      <c r="H125" s="17"/>
+      <c r="I125" s="17"/>
+      <c r="J125" s="17"/>
+      <c r="K125" s="17"/>
+      <c r="L125" s="17"/>
+      <c r="M125" s="17"/>
+      <c r="N125" s="17"/>
+      <c r="O125" s="17"/>
+      <c r="P125" s="17"/>
+      <c r="Q125" s="17"/>
+      <c r="R125" s="17"/>
+      <c r="S125" s="17"/>
+      <c r="T125" s="9"/>
+    </row>
+    <row r="126" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B126" s="8"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="17"/>
+      <c r="G126" s="17"/>
+      <c r="H126" s="17"/>
+      <c r="I126" s="17"/>
+      <c r="J126" s="17"/>
+      <c r="K126" s="17"/>
+      <c r="L126" s="17"/>
+      <c r="M126" s="17"/>
+      <c r="N126" s="17"/>
+      <c r="O126" s="17"/>
+      <c r="P126" s="17"/>
+      <c r="Q126" s="17"/>
+      <c r="R126" s="17"/>
+      <c r="S126" s="17"/>
+      <c r="T126" s="9"/>
+    </row>
+    <row r="127" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B127" s="8"/>
+      <c r="C127" s="17"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="17"/>
+      <c r="G127" s="17"/>
+      <c r="H127" s="17"/>
+      <c r="I127" s="17"/>
+      <c r="J127" s="17"/>
+      <c r="K127" s="17"/>
+      <c r="L127" s="17"/>
+      <c r="M127" s="17"/>
+      <c r="N127" s="17"/>
+      <c r="O127" s="17"/>
+      <c r="P127" s="17"/>
+      <c r="Q127" s="17"/>
+      <c r="R127" s="17"/>
+      <c r="S127" s="17"/>
+      <c r="T127" s="9"/>
+    </row>
+    <row r="128" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B128" s="8"/>
+      <c r="C128" s="17"/>
+      <c r="D128" s="17"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="17"/>
+      <c r="G128" s="17"/>
+      <c r="H128" s="17"/>
+      <c r="I128" s="17"/>
+      <c r="J128" s="17"/>
+      <c r="K128" s="17"/>
+      <c r="L128" s="17"/>
+      <c r="M128" s="17"/>
+      <c r="N128" s="17"/>
+      <c r="O128" s="17"/>
+      <c r="P128" s="17"/>
+      <c r="Q128" s="17"/>
+      <c r="R128" s="17"/>
+      <c r="S128" s="17"/>
+      <c r="T128" s="9"/>
+    </row>
+    <row r="129" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B129" s="8"/>
+      <c r="C129" s="17"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="17"/>
+      <c r="G129" s="17"/>
+      <c r="H129" s="17"/>
+      <c r="I129" s="17"/>
+      <c r="J129" s="17"/>
+      <c r="K129" s="17"/>
+      <c r="L129" s="17"/>
+      <c r="M129" s="17"/>
+      <c r="N129" s="17"/>
+      <c r="O129" s="17"/>
+      <c r="P129" s="17"/>
+      <c r="Q129" s="17"/>
+      <c r="R129" s="17"/>
+      <c r="S129" s="17"/>
+      <c r="T129" s="9"/>
+    </row>
+    <row r="130" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B130" s="8"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="17"/>
+      <c r="G130" s="17"/>
+      <c r="H130" s="17"/>
+      <c r="I130" s="17"/>
+      <c r="J130" s="17"/>
+      <c r="K130" s="17"/>
+      <c r="L130" s="17"/>
+      <c r="M130" s="17"/>
+      <c r="N130" s="17"/>
+      <c r="O130" s="17"/>
+      <c r="P130" s="17"/>
+      <c r="Q130" s="17"/>
+      <c r="R130" s="17"/>
+      <c r="S130" s="17"/>
+      <c r="T130" s="9"/>
+    </row>
+    <row r="131" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B131" s="8"/>
+      <c r="C131" s="17"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="17"/>
+      <c r="G131" s="17"/>
+      <c r="H131" s="17"/>
+      <c r="I131" s="17"/>
+      <c r="J131" s="17"/>
+      <c r="K131" s="17"/>
+      <c r="L131" s="17"/>
+      <c r="M131" s="17"/>
+      <c r="N131" s="17"/>
+      <c r="O131" s="17"/>
+      <c r="P131" s="17"/>
+      <c r="Q131" s="17"/>
+      <c r="R131" s="17"/>
+      <c r="S131" s="17"/>
+      <c r="T131" s="9"/>
+    </row>
+    <row r="132" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B132" s="8"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="17"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="17"/>
+      <c r="G132" s="17"/>
+      <c r="H132" s="17"/>
+      <c r="I132" s="17"/>
+      <c r="J132" s="17"/>
+      <c r="K132" s="17"/>
+      <c r="L132" s="17"/>
+      <c r="M132" s="17"/>
+      <c r="N132" s="17"/>
+      <c r="O132" s="17"/>
+      <c r="P132" s="17"/>
+      <c r="Q132" s="17"/>
+      <c r="R132" s="17"/>
+      <c r="S132" s="17"/>
+      <c r="T132" s="9"/>
+    </row>
+    <row r="133" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B133" s="8"/>
+      <c r="C133" s="17"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="17"/>
+      <c r="G133" s="17"/>
+      <c r="H133" s="17"/>
+      <c r="I133" s="17"/>
+      <c r="J133" s="17"/>
+      <c r="K133" s="17"/>
+      <c r="L133" s="17"/>
+      <c r="M133" s="17"/>
+      <c r="N133" s="17"/>
+      <c r="O133" s="17"/>
+      <c r="P133" s="17"/>
+      <c r="Q133" s="17"/>
+      <c r="R133" s="17"/>
+      <c r="S133" s="17"/>
+      <c r="T133" s="9"/>
+    </row>
+    <row r="134" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B134" s="8"/>
+      <c r="C134" s="17"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="17"/>
+      <c r="G134" s="17"/>
+      <c r="H134" s="17"/>
+      <c r="I134" s="17"/>
+      <c r="J134" s="17"/>
+      <c r="K134" s="17"/>
+      <c r="L134" s="17"/>
+      <c r="M134" s="17"/>
+      <c r="N134" s="17"/>
+      <c r="O134" s="17"/>
+      <c r="P134" s="17"/>
+      <c r="Q134" s="17"/>
+      <c r="R134" s="17"/>
+      <c r="S134" s="17"/>
+      <c r="T134" s="9"/>
+    </row>
+    <row r="135" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B135" s="8"/>
+      <c r="C135" s="17"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="17"/>
+      <c r="G135" s="17"/>
+      <c r="H135" s="17"/>
+      <c r="I135" s="17"/>
+      <c r="J135" s="17"/>
+      <c r="K135" s="17"/>
+      <c r="L135" s="17"/>
+      <c r="M135" s="17"/>
+      <c r="N135" s="17"/>
+      <c r="O135" s="17"/>
+      <c r="P135" s="17"/>
+      <c r="Q135" s="17"/>
+      <c r="R135" s="17"/>
+      <c r="S135" s="17"/>
+      <c r="T135" s="9"/>
+    </row>
+    <row r="136" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B136" s="8"/>
+      <c r="C136" s="17"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="17"/>
+      <c r="G136" s="17"/>
+      <c r="H136" s="17"/>
+      <c r="I136" s="17"/>
+      <c r="J136" s="17"/>
+      <c r="K136" s="17"/>
+      <c r="L136" s="17"/>
+      <c r="M136" s="17"/>
+      <c r="N136" s="17"/>
+      <c r="O136" s="17"/>
+      <c r="P136" s="17"/>
+      <c r="Q136" s="17"/>
+      <c r="R136" s="17"/>
+      <c r="S136" s="17"/>
+      <c r="T136" s="9"/>
+    </row>
+    <row r="137" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B137" s="8"/>
+      <c r="C137" s="17"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="17"/>
+      <c r="H137" s="17"/>
+      <c r="I137" s="17"/>
+      <c r="J137" s="17"/>
+      <c r="K137" s="17"/>
+      <c r="L137" s="17"/>
+      <c r="M137" s="17"/>
+      <c r="N137" s="17"/>
+      <c r="O137" s="17"/>
+      <c r="P137" s="17"/>
+      <c r="Q137" s="17"/>
+      <c r="R137" s="17"/>
+      <c r="S137" s="17"/>
+      <c r="T137" s="9"/>
+    </row>
+    <row r="138" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B138" s="8"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
+      <c r="H138" s="17"/>
+      <c r="I138" s="17"/>
+      <c r="J138" s="17"/>
+      <c r="K138" s="17"/>
+      <c r="L138" s="17"/>
+      <c r="M138" s="17"/>
+      <c r="N138" s="17"/>
+      <c r="O138" s="17"/>
+      <c r="P138" s="17"/>
+      <c r="Q138" s="17"/>
+      <c r="R138" s="17"/>
+      <c r="S138" s="17"/>
+      <c r="T138" s="9"/>
+    </row>
+    <row r="139" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B139" s="8"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="17"/>
+      <c r="G139" s="17"/>
+      <c r="H139" s="17"/>
+      <c r="I139" s="17"/>
+      <c r="J139" s="17"/>
+      <c r="K139" s="17"/>
+      <c r="L139" s="17"/>
+      <c r="M139" s="17"/>
+      <c r="N139" s="17"/>
+      <c r="O139" s="17"/>
+      <c r="P139" s="17"/>
+      <c r="Q139" s="17"/>
+      <c r="R139" s="17"/>
+      <c r="S139" s="17"/>
+      <c r="T139" s="9"/>
+    </row>
+    <row r="140" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B140" s="8"/>
+      <c r="C140" s="17"/>
+      <c r="D140" s="17"/>
+      <c r="E140" s="17"/>
+      <c r="F140" s="17"/>
+      <c r="G140" s="17"/>
+      <c r="H140" s="17"/>
+      <c r="I140" s="17"/>
+      <c r="J140" s="17"/>
+      <c r="K140" s="17"/>
+      <c r="L140" s="17"/>
+      <c r="M140" s="17"/>
+      <c r="N140" s="17"/>
+      <c r="O140" s="17"/>
+      <c r="P140" s="17"/>
+      <c r="Q140" s="17"/>
+      <c r="R140" s="17"/>
+      <c r="S140" s="17"/>
+      <c r="T140" s="9"/>
+    </row>
+    <row r="141" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B141" s="10"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="5"/>
+      <c r="J141" s="5"/>
+      <c r="K141" s="5"/>
+      <c r="L141" s="5"/>
+      <c r="M141" s="5"/>
+      <c r="N141" s="5"/>
+      <c r="O141" s="5"/>
+      <c r="P141" s="5"/>
+      <c r="Q141" s="5"/>
+      <c r="R141" s="5"/>
+      <c r="S141" s="5"/>
+      <c r="T141" s="6"/>
+    </row>
+    <row r="144" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B144" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+      <c r="J144" s="2"/>
+      <c r="K144" s="2"/>
+      <c r="L144" s="2"/>
+      <c r="M144" s="2"/>
+      <c r="N144" s="2"/>
+      <c r="O144" s="2"/>
+      <c r="P144" s="2"/>
+      <c r="Q144" s="2"/>
+      <c r="R144" s="2"/>
+      <c r="S144" s="2"/>
+      <c r="T144" s="3"/>
+    </row>
+    <row r="145" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B145" s="8"/>
+      <c r="C145" s="17"/>
+      <c r="D145" s="17"/>
+      <c r="E145" s="17"/>
+      <c r="F145" s="17"/>
+      <c r="G145" s="17"/>
+      <c r="H145" s="17"/>
+      <c r="I145" s="17"/>
+      <c r="J145" s="17"/>
+      <c r="K145" s="17"/>
+      <c r="L145" s="17"/>
+      <c r="M145" s="17"/>
+      <c r="N145" s="17"/>
+      <c r="O145" s="17"/>
+      <c r="P145" s="17"/>
+      <c r="Q145" s="17"/>
+      <c r="R145" s="17"/>
+      <c r="S145" s="17"/>
+      <c r="T145" s="9"/>
+    </row>
+    <row r="146" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B146" s="8"/>
+      <c r="C146" s="17"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="17"/>
+      <c r="F146" s="17"/>
+      <c r="G146" s="17"/>
+      <c r="H146" s="17"/>
+      <c r="I146" s="17"/>
+      <c r="J146" s="17"/>
+      <c r="K146" s="17"/>
+      <c r="L146" s="17"/>
+      <c r="M146" s="17"/>
+      <c r="N146" s="17"/>
+      <c r="O146" s="17"/>
+      <c r="P146" s="17"/>
+      <c r="Q146" s="17"/>
+      <c r="R146" s="17"/>
+      <c r="S146" s="17"/>
+      <c r="T146" s="9"/>
+    </row>
+    <row r="147" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B147" s="8"/>
+      <c r="C147" s="17"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="17"/>
+      <c r="G147" s="17"/>
+      <c r="H147" s="17"/>
+      <c r="I147" s="17"/>
+      <c r="J147" s="17"/>
+      <c r="K147" s="17"/>
+      <c r="L147" s="17"/>
+      <c r="M147" s="17"/>
+      <c r="N147" s="17"/>
+      <c r="O147" s="17"/>
+      <c r="P147" s="17"/>
+      <c r="Q147" s="17"/>
+      <c r="R147" s="17"/>
+      <c r="S147" s="17"/>
+      <c r="T147" s="9"/>
+    </row>
+    <row r="148" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B148" s="8"/>
+      <c r="C148" s="17"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="17"/>
+      <c r="G148" s="17"/>
+      <c r="H148" s="17"/>
+      <c r="I148" s="17"/>
+      <c r="J148" s="17"/>
+      <c r="K148" s="17"/>
+      <c r="L148" s="17"/>
+      <c r="M148" s="17"/>
+      <c r="N148" s="17"/>
+      <c r="O148" s="17"/>
+      <c r="P148" s="17"/>
+      <c r="Q148" s="17"/>
+      <c r="R148" s="17"/>
+      <c r="S148" s="17"/>
+      <c r="T148" s="9"/>
+    </row>
+    <row r="149" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B149" s="8"/>
+      <c r="C149" s="17"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="17"/>
+      <c r="G149" s="17"/>
+      <c r="H149" s="17"/>
+      <c r="I149" s="17"/>
+      <c r="J149" s="17"/>
+      <c r="K149" s="17"/>
+      <c r="L149" s="17"/>
+      <c r="M149" s="17"/>
+      <c r="N149" s="17"/>
+      <c r="O149" s="17"/>
+      <c r="P149" s="17"/>
+      <c r="Q149" s="17"/>
+      <c r="R149" s="17"/>
+      <c r="S149" s="17"/>
+      <c r="T149" s="9"/>
+    </row>
+    <row r="150" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B150" s="8"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="17"/>
+      <c r="G150" s="17"/>
+      <c r="H150" s="17"/>
+      <c r="I150" s="17"/>
+      <c r="J150" s="17"/>
+      <c r="K150" s="17"/>
+      <c r="L150" s="17"/>
+      <c r="M150" s="17"/>
+      <c r="N150" s="17"/>
+      <c r="O150" s="17"/>
+      <c r="P150" s="17"/>
+      <c r="Q150" s="17"/>
+      <c r="R150" s="17"/>
+      <c r="S150" s="17"/>
+      <c r="T150" s="9"/>
+    </row>
+    <row r="151" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B151" s="8"/>
+      <c r="C151" s="17"/>
+      <c r="D151" s="17"/>
+      <c r="E151" s="17"/>
+      <c r="F151" s="17"/>
+      <c r="G151" s="17"/>
+      <c r="H151" s="17"/>
+      <c r="I151" s="17"/>
+      <c r="J151" s="17"/>
+      <c r="K151" s="17"/>
+      <c r="L151" s="17"/>
+      <c r="M151" s="17"/>
+      <c r="N151" s="17"/>
+      <c r="O151" s="17"/>
+      <c r="P151" s="17"/>
+      <c r="Q151" s="17"/>
+      <c r="R151" s="17"/>
+      <c r="S151" s="17"/>
+      <c r="T151" s="9"/>
+    </row>
+    <row r="152" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B152" s="8"/>
+      <c r="C152" s="17"/>
+      <c r="D152" s="17"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="17"/>
+      <c r="G152" s="17"/>
+      <c r="H152" s="17"/>
+      <c r="I152" s="17"/>
+      <c r="J152" s="17"/>
+      <c r="K152" s="17"/>
+      <c r="L152" s="17"/>
+      <c r="M152" s="17"/>
+      <c r="N152" s="17"/>
+      <c r="O152" s="17"/>
+      <c r="P152" s="17"/>
+      <c r="Q152" s="17"/>
+      <c r="R152" s="17"/>
+      <c r="S152" s="17"/>
+      <c r="T152" s="9"/>
+    </row>
+    <row r="153" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B153" s="8"/>
+      <c r="C153" s="17"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="17"/>
+      <c r="G153" s="17"/>
+      <c r="H153" s="17"/>
+      <c r="I153" s="17"/>
+      <c r="J153" s="17"/>
+      <c r="K153" s="17"/>
+      <c r="L153" s="17"/>
+      <c r="M153" s="17"/>
+      <c r="N153" s="17"/>
+      <c r="O153" s="17"/>
+      <c r="P153" s="17"/>
+      <c r="Q153" s="17"/>
+      <c r="R153" s="17"/>
+      <c r="S153" s="17"/>
+      <c r="T153" s="9"/>
+    </row>
+    <row r="154" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B154" s="8"/>
+      <c r="C154" s="17"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="17"/>
+      <c r="G154" s="17"/>
+      <c r="H154" s="17"/>
+      <c r="I154" s="17"/>
+      <c r="J154" s="17"/>
+      <c r="K154" s="17"/>
+      <c r="L154" s="17"/>
+      <c r="M154" s="17"/>
+      <c r="N154" s="17"/>
+      <c r="O154" s="17"/>
+      <c r="P154" s="17"/>
+      <c r="Q154" s="17"/>
+      <c r="R154" s="17"/>
+      <c r="S154" s="17"/>
+      <c r="T154" s="9"/>
+    </row>
+    <row r="155" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B155" s="8"/>
+      <c r="C155" s="17"/>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="17"/>
+      <c r="G155" s="17"/>
+      <c r="H155" s="17"/>
+      <c r="I155" s="17"/>
+      <c r="J155" s="17"/>
+      <c r="K155" s="17"/>
+      <c r="L155" s="17"/>
+      <c r="M155" s="17"/>
+      <c r="N155" s="17"/>
+      <c r="O155" s="17"/>
+      <c r="P155" s="17"/>
+      <c r="Q155" s="17"/>
+      <c r="R155" s="17"/>
+      <c r="S155" s="17"/>
+      <c r="T155" s="9"/>
+    </row>
+    <row r="156" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B156" s="8"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="17"/>
+      <c r="E156" s="17"/>
+      <c r="F156" s="17"/>
+      <c r="G156" s="17"/>
+      <c r="H156" s="17"/>
+      <c r="I156" s="17"/>
+      <c r="J156" s="17"/>
+      <c r="K156" s="17"/>
+      <c r="L156" s="17"/>
+      <c r="M156" s="17"/>
+      <c r="N156" s="17"/>
+      <c r="O156" s="17"/>
+      <c r="P156" s="17"/>
+      <c r="Q156" s="17"/>
+      <c r="R156" s="17"/>
+      <c r="S156" s="17"/>
+      <c r="T156" s="9"/>
+    </row>
+    <row r="157" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B157" s="8"/>
+      <c r="C157" s="17"/>
+      <c r="D157" s="17"/>
+      <c r="E157" s="17"/>
+      <c r="F157" s="17"/>
+      <c r="G157" s="17"/>
+      <c r="H157" s="17"/>
+      <c r="I157" s="17"/>
+      <c r="J157" s="17"/>
+      <c r="K157" s="17"/>
+      <c r="L157" s="17"/>
+      <c r="M157" s="17"/>
+      <c r="N157" s="17"/>
+      <c r="O157" s="17"/>
+      <c r="P157" s="17"/>
+      <c r="Q157" s="17"/>
+      <c r="R157" s="17"/>
+      <c r="S157" s="17"/>
+      <c r="T157" s="9"/>
+    </row>
+    <row r="158" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B158" s="8"/>
+      <c r="C158" s="17"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="17"/>
+      <c r="G158" s="17"/>
+      <c r="H158" s="17"/>
+      <c r="I158" s="17"/>
+      <c r="J158" s="17"/>
+      <c r="K158" s="17"/>
+      <c r="L158" s="17"/>
+      <c r="M158" s="17"/>
+      <c r="N158" s="17"/>
+      <c r="O158" s="17"/>
+      <c r="P158" s="17"/>
+      <c r="Q158" s="17"/>
+      <c r="R158" s="17"/>
+      <c r="S158" s="17"/>
+      <c r="T158" s="9"/>
+    </row>
+    <row r="159" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B159" s="8"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="17"/>
+      <c r="G159" s="17"/>
+      <c r="H159" s="17"/>
+      <c r="I159" s="17"/>
+      <c r="J159" s="17"/>
+      <c r="K159" s="17"/>
+      <c r="L159" s="17"/>
+      <c r="M159" s="17"/>
+      <c r="N159" s="17"/>
+      <c r="O159" s="17"/>
+      <c r="P159" s="17"/>
+      <c r="Q159" s="17"/>
+      <c r="R159" s="17"/>
+      <c r="S159" s="17"/>
+      <c r="T159" s="9"/>
+    </row>
+    <row r="160" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B160" s="8"/>
+      <c r="C160" s="17"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="17"/>
+      <c r="G160" s="17"/>
+      <c r="H160" s="17"/>
+      <c r="I160" s="17"/>
+      <c r="J160" s="17"/>
+      <c r="K160" s="17"/>
+      <c r="L160" s="17"/>
+      <c r="M160" s="17"/>
+      <c r="N160" s="17"/>
+      <c r="O160" s="17"/>
+      <c r="P160" s="17"/>
+      <c r="Q160" s="17"/>
+      <c r="R160" s="17"/>
+      <c r="S160" s="17"/>
+      <c r="T160" s="9"/>
+    </row>
+    <row r="161" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B161" s="8"/>
+      <c r="C161" s="17"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="17"/>
+      <c r="G161" s="17"/>
+      <c r="H161" s="17"/>
+      <c r="I161" s="17"/>
+      <c r="J161" s="17"/>
+      <c r="K161" s="17"/>
+      <c r="L161" s="17"/>
+      <c r="M161" s="17"/>
+      <c r="N161" s="17"/>
+      <c r="O161" s="17"/>
+      <c r="P161" s="17"/>
+      <c r="Q161" s="17"/>
+      <c r="R161" s="17"/>
+      <c r="S161" s="17"/>
+      <c r="T161" s="9"/>
+    </row>
+    <row r="162" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B162" s="8"/>
+      <c r="C162" s="17"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="17"/>
+      <c r="G162" s="17"/>
+      <c r="H162" s="17"/>
+      <c r="I162" s="17"/>
+      <c r="J162" s="17"/>
+      <c r="K162" s="17"/>
+      <c r="L162" s="17"/>
+      <c r="M162" s="17"/>
+      <c r="N162" s="17"/>
+      <c r="O162" s="17"/>
+      <c r="P162" s="17"/>
+      <c r="Q162" s="17"/>
+      <c r="R162" s="17"/>
+      <c r="S162" s="17"/>
+      <c r="T162" s="9"/>
+    </row>
+    <row r="163" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B163" s="8"/>
+      <c r="C163" s="17"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="17"/>
+      <c r="G163" s="17"/>
+      <c r="H163" s="17"/>
+      <c r="I163" s="17"/>
+      <c r="J163" s="17"/>
+      <c r="K163" s="17"/>
+      <c r="L163" s="17"/>
+      <c r="M163" s="17"/>
+      <c r="N163" s="17"/>
+      <c r="O163" s="17"/>
+      <c r="P163" s="17"/>
+      <c r="Q163" s="17"/>
+      <c r="R163" s="17"/>
+      <c r="S163" s="17"/>
+      <c r="T163" s="9"/>
+    </row>
+    <row r="164" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B164" s="8"/>
+      <c r="C164" s="17"/>
+      <c r="D164" s="17"/>
+      <c r="E164" s="17"/>
+      <c r="F164" s="17"/>
+      <c r="G164" s="17"/>
+      <c r="H164" s="17"/>
+      <c r="I164" s="17"/>
+      <c r="J164" s="17"/>
+      <c r="K164" s="17"/>
+      <c r="L164" s="17"/>
+      <c r="M164" s="17"/>
+      <c r="N164" s="17"/>
+      <c r="O164" s="17"/>
+      <c r="P164" s="17"/>
+      <c r="Q164" s="17"/>
+      <c r="R164" s="17"/>
+      <c r="S164" s="17"/>
+      <c r="T164" s="9"/>
+    </row>
+    <row r="165" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B165" s="8"/>
+      <c r="C165" s="17"/>
+      <c r="D165" s="17"/>
+      <c r="E165" s="17"/>
+      <c r="F165" s="17"/>
+      <c r="G165" s="17"/>
+      <c r="H165" s="17"/>
+      <c r="I165" s="17"/>
+      <c r="J165" s="17"/>
+      <c r="K165" s="17"/>
+      <c r="L165" s="17"/>
+      <c r="M165" s="17"/>
+      <c r="N165" s="17"/>
+      <c r="O165" s="17"/>
+      <c r="P165" s="17"/>
+      <c r="Q165" s="17"/>
+      <c r="R165" s="17"/>
+      <c r="S165" s="17"/>
+      <c r="T165" s="9"/>
+    </row>
+    <row r="166" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B166" s="8"/>
+      <c r="C166" s="17"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="17"/>
+      <c r="G166" s="17"/>
+      <c r="H166" s="17"/>
+      <c r="I166" s="17"/>
+      <c r="J166" s="17"/>
+      <c r="K166" s="17"/>
+      <c r="L166" s="17"/>
+      <c r="M166" s="17"/>
+      <c r="N166" s="17"/>
+      <c r="O166" s="17"/>
+      <c r="P166" s="17"/>
+      <c r="Q166" s="17"/>
+      <c r="R166" s="17"/>
+      <c r="S166" s="17"/>
+      <c r="T166" s="9"/>
+    </row>
+    <row r="167" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B167" s="8"/>
+      <c r="C167" s="17"/>
+      <c r="D167" s="17"/>
+      <c r="E167" s="17"/>
+      <c r="F167" s="17"/>
+      <c r="G167" s="17"/>
+      <c r="H167" s="17"/>
+      <c r="I167" s="17"/>
+      <c r="J167" s="17"/>
+      <c r="K167" s="17"/>
+      <c r="L167" s="17"/>
+      <c r="M167" s="17"/>
+      <c r="N167" s="17"/>
+      <c r="O167" s="17"/>
+      <c r="P167" s="17"/>
+      <c r="Q167" s="17"/>
+      <c r="R167" s="17"/>
+      <c r="S167" s="17"/>
+      <c r="T167" s="9"/>
+    </row>
+    <row r="168" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B168" s="8"/>
+      <c r="C168" s="17"/>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17"/>
+      <c r="F168" s="17"/>
+      <c r="G168" s="17"/>
+      <c r="H168" s="17"/>
+      <c r="I168" s="17"/>
+      <c r="J168" s="17"/>
+      <c r="K168" s="17"/>
+      <c r="L168" s="17"/>
+      <c r="M168" s="17"/>
+      <c r="N168" s="17"/>
+      <c r="O168" s="17"/>
+      <c r="P168" s="17"/>
+      <c r="Q168" s="17"/>
+      <c r="R168" s="17"/>
+      <c r="S168" s="17"/>
+      <c r="T168" s="9"/>
+    </row>
+    <row r="169" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B169" s="8"/>
+      <c r="C169" s="17"/>
+      <c r="D169" s="17"/>
+      <c r="E169" s="17"/>
+      <c r="F169" s="17"/>
+      <c r="G169" s="17"/>
+      <c r="H169" s="17"/>
+      <c r="I169" s="17"/>
+      <c r="J169" s="17"/>
+      <c r="K169" s="17"/>
+      <c r="L169" s="17"/>
+      <c r="M169" s="17"/>
+      <c r="N169" s="17"/>
+      <c r="O169" s="17"/>
+      <c r="P169" s="17"/>
+      <c r="Q169" s="17"/>
+      <c r="R169" s="17"/>
+      <c r="S169" s="17"/>
+      <c r="T169" s="9"/>
+    </row>
+    <row r="170" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B170" s="8"/>
+      <c r="C170" s="17"/>
+      <c r="D170" s="17"/>
+      <c r="E170" s="17"/>
+      <c r="F170" s="17"/>
+      <c r="G170" s="17"/>
+      <c r="H170" s="17"/>
+      <c r="I170" s="17"/>
+      <c r="J170" s="17"/>
+      <c r="K170" s="17"/>
+      <c r="L170" s="17"/>
+      <c r="M170" s="17"/>
+      <c r="N170" s="17"/>
+      <c r="O170" s="17"/>
+      <c r="P170" s="17"/>
+      <c r="Q170" s="17"/>
+      <c r="R170" s="17"/>
+      <c r="S170" s="17"/>
+      <c r="T170" s="9"/>
+    </row>
+    <row r="171" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B171" s="8"/>
+      <c r="C171" s="17"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="17"/>
+      <c r="F171" s="17"/>
+      <c r="G171" s="17"/>
+      <c r="H171" s="17"/>
+      <c r="I171" s="17"/>
+      <c r="J171" s="17"/>
+      <c r="K171" s="17"/>
+      <c r="L171" s="17"/>
+      <c r="M171" s="17"/>
+      <c r="N171" s="17"/>
+      <c r="O171" s="17"/>
+      <c r="P171" s="17"/>
+      <c r="Q171" s="17"/>
+      <c r="R171" s="17"/>
+      <c r="S171" s="17"/>
+      <c r="T171" s="9"/>
+    </row>
+    <row r="172" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B172" s="8"/>
+      <c r="C172" s="17"/>
+      <c r="D172" s="17"/>
+      <c r="E172" s="17"/>
+      <c r="F172" s="17"/>
+      <c r="G172" s="17"/>
+      <c r="H172" s="17"/>
+      <c r="I172" s="17"/>
+      <c r="J172" s="17"/>
+      <c r="K172" s="17"/>
+      <c r="L172" s="17"/>
+      <c r="M172" s="17"/>
+      <c r="N172" s="17"/>
+      <c r="O172" s="17"/>
+      <c r="P172" s="17"/>
+      <c r="Q172" s="17"/>
+      <c r="R172" s="17"/>
+      <c r="S172" s="17"/>
+      <c r="T172" s="9"/>
+    </row>
+    <row r="173" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B173" s="8"/>
+      <c r="C173" s="17"/>
+      <c r="D173" s="17"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="17"/>
+      <c r="G173" s="17"/>
+      <c r="H173" s="17"/>
+      <c r="I173" s="17"/>
+      <c r="J173" s="17"/>
+      <c r="K173" s="17"/>
+      <c r="L173" s="17"/>
+      <c r="M173" s="17"/>
+      <c r="N173" s="17"/>
+      <c r="O173" s="17"/>
+      <c r="P173" s="17"/>
+      <c r="Q173" s="17"/>
+      <c r="R173" s="17"/>
+      <c r="S173" s="17"/>
+      <c r="T173" s="9"/>
+    </row>
+    <row r="174" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B174" s="8"/>
+      <c r="C174" s="17"/>
+      <c r="D174" s="17"/>
+      <c r="E174" s="17"/>
+      <c r="F174" s="17"/>
+      <c r="G174" s="17"/>
+      <c r="H174" s="17"/>
+      <c r="I174" s="17"/>
+      <c r="J174" s="17"/>
+      <c r="K174" s="17"/>
+      <c r="L174" s="17"/>
+      <c r="M174" s="17"/>
+      <c r="N174" s="17"/>
+      <c r="O174" s="17"/>
+      <c r="P174" s="17"/>
+      <c r="Q174" s="17"/>
+      <c r="R174" s="17"/>
+      <c r="S174" s="17"/>
+      <c r="T174" s="9"/>
+    </row>
+    <row r="175" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B175" s="8"/>
+      <c r="C175" s="17"/>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="17"/>
+      <c r="G175" s="17"/>
+      <c r="H175" s="17"/>
+      <c r="I175" s="17"/>
+      <c r="J175" s="17"/>
+      <c r="K175" s="17"/>
+      <c r="L175" s="17"/>
+      <c r="M175" s="17"/>
+      <c r="N175" s="17"/>
+      <c r="O175" s="17"/>
+      <c r="P175" s="17"/>
+      <c r="Q175" s="17"/>
+      <c r="R175" s="17"/>
+      <c r="S175" s="17"/>
+      <c r="T175" s="9"/>
+    </row>
+    <row r="176" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B176" s="8"/>
+      <c r="C176" s="17"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="17"/>
+      <c r="F176" s="17"/>
+      <c r="G176" s="17"/>
+      <c r="H176" s="17"/>
+      <c r="I176" s="17"/>
+      <c r="J176" s="17"/>
+      <c r="K176" s="17"/>
+      <c r="L176" s="17"/>
+      <c r="M176" s="17"/>
+      <c r="N176" s="17"/>
+      <c r="O176" s="17"/>
+      <c r="P176" s="17"/>
+      <c r="Q176" s="17"/>
+      <c r="R176" s="17"/>
+      <c r="S176" s="17"/>
+      <c r="T176" s="9"/>
+    </row>
+    <row r="177" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B177" s="8"/>
+      <c r="C177" s="17"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="17"/>
+      <c r="G177" s="17"/>
+      <c r="H177" s="17"/>
+      <c r="I177" s="17"/>
+      <c r="J177" s="17"/>
+      <c r="K177" s="17"/>
+      <c r="L177" s="17"/>
+      <c r="M177" s="17"/>
+      <c r="N177" s="17"/>
+      <c r="O177" s="17"/>
+      <c r="P177" s="17"/>
+      <c r="Q177" s="17"/>
+      <c r="R177" s="17"/>
+      <c r="S177" s="17"/>
+      <c r="T177" s="9"/>
+    </row>
+    <row r="178" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B178" s="8"/>
+      <c r="C178" s="17"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="17"/>
+      <c r="G178" s="17"/>
+      <c r="H178" s="17"/>
+      <c r="I178" s="17"/>
+      <c r="J178" s="17"/>
+      <c r="K178" s="17"/>
+      <c r="L178" s="17"/>
+      <c r="M178" s="17"/>
+      <c r="N178" s="17"/>
+      <c r="O178" s="17"/>
+      <c r="P178" s="17"/>
+      <c r="Q178" s="17"/>
+      <c r="R178" s="17"/>
+      <c r="S178" s="17"/>
+      <c r="T178" s="9"/>
+    </row>
+    <row r="179" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B179" s="8"/>
+      <c r="C179" s="17"/>
+      <c r="D179" s="17"/>
+      <c r="E179" s="17"/>
+      <c r="F179" s="17"/>
+      <c r="G179" s="17"/>
+      <c r="H179" s="17"/>
+      <c r="I179" s="17"/>
+      <c r="J179" s="17"/>
+      <c r="K179" s="17"/>
+      <c r="L179" s="17"/>
+      <c r="M179" s="17"/>
+      <c r="N179" s="17"/>
+      <c r="O179" s="17"/>
+      <c r="P179" s="17"/>
+      <c r="Q179" s="17"/>
+      <c r="R179" s="17"/>
+      <c r="S179" s="17"/>
+      <c r="T179" s="9"/>
+    </row>
+    <row r="180" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B180" s="8"/>
+      <c r="C180" s="17"/>
+      <c r="D180" s="17"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="17"/>
+      <c r="G180" s="17"/>
+      <c r="H180" s="17"/>
+      <c r="I180" s="17"/>
+      <c r="J180" s="17"/>
+      <c r="K180" s="17"/>
+      <c r="L180" s="17"/>
+      <c r="M180" s="17"/>
+      <c r="N180" s="17"/>
+      <c r="O180" s="17"/>
+      <c r="P180" s="17"/>
+      <c r="Q180" s="17"/>
+      <c r="R180" s="17"/>
+      <c r="S180" s="17"/>
+      <c r="T180" s="9"/>
+    </row>
+    <row r="181" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B181" s="8"/>
+      <c r="C181" s="17"/>
+      <c r="D181" s="17"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="17"/>
+      <c r="G181" s="17"/>
+      <c r="H181" s="17"/>
+      <c r="I181" s="17"/>
+      <c r="J181" s="17"/>
+      <c r="K181" s="17"/>
+      <c r="L181" s="17"/>
+      <c r="M181" s="17"/>
+      <c r="N181" s="17"/>
+      <c r="O181" s="17"/>
+      <c r="P181" s="17"/>
+      <c r="Q181" s="17"/>
+      <c r="R181" s="17"/>
+      <c r="S181" s="17"/>
+      <c r="T181" s="9"/>
+    </row>
+    <row r="182" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B182" s="8"/>
+      <c r="C182" s="17"/>
+      <c r="D182" s="17"/>
+      <c r="E182" s="17"/>
+      <c r="F182" s="17"/>
+      <c r="G182" s="17"/>
+      <c r="H182" s="17"/>
+      <c r="I182" s="17"/>
+      <c r="J182" s="17"/>
+      <c r="K182" s="17"/>
+      <c r="L182" s="17"/>
+      <c r="M182" s="17"/>
+      <c r="N182" s="17"/>
+      <c r="O182" s="17"/>
+      <c r="P182" s="17"/>
+      <c r="Q182" s="17"/>
+      <c r="R182" s="17"/>
+      <c r="S182" s="17"/>
+      <c r="T182" s="9"/>
+    </row>
+    <row r="183" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B183" s="8"/>
+      <c r="C183" s="17"/>
+      <c r="D183" s="17"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="17"/>
+      <c r="G183" s="17"/>
+      <c r="H183" s="17"/>
+      <c r="I183" s="17"/>
+      <c r="J183" s="17"/>
+      <c r="K183" s="17"/>
+      <c r="L183" s="17"/>
+      <c r="M183" s="17"/>
+      <c r="N183" s="17"/>
+      <c r="O183" s="17"/>
+      <c r="P183" s="17"/>
+      <c r="Q183" s="17"/>
+      <c r="R183" s="17"/>
+      <c r="S183" s="17"/>
+      <c r="T183" s="9"/>
+    </row>
+    <row r="184" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B184" s="8"/>
+      <c r="C184" s="17"/>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="17"/>
+      <c r="G184" s="17"/>
+      <c r="H184" s="17"/>
+      <c r="I184" s="17"/>
+      <c r="J184" s="17"/>
+      <c r="K184" s="17"/>
+      <c r="L184" s="17"/>
+      <c r="M184" s="17"/>
+      <c r="N184" s="17"/>
+      <c r="O184" s="17"/>
+      <c r="P184" s="17"/>
+      <c r="Q184" s="17"/>
+      <c r="R184" s="17"/>
+      <c r="S184" s="17"/>
+      <c r="T184" s="9"/>
+    </row>
+    <row r="185" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B185" s="8"/>
+      <c r="C185" s="17"/>
+      <c r="D185" s="17"/>
+      <c r="E185" s="17"/>
+      <c r="F185" s="17"/>
+      <c r="G185" s="17"/>
+      <c r="H185" s="17"/>
+      <c r="I185" s="17"/>
+      <c r="J185" s="17"/>
+      <c r="K185" s="17"/>
+      <c r="L185" s="17"/>
+      <c r="M185" s="17"/>
+      <c r="N185" s="17"/>
+      <c r="O185" s="17"/>
+      <c r="P185" s="17"/>
+      <c r="Q185" s="17"/>
+      <c r="R185" s="17"/>
+      <c r="S185" s="17"/>
+      <c r="T185" s="9"/>
+    </row>
+    <row r="186" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B186" s="8"/>
+      <c r="C186" s="17"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="17"/>
+      <c r="G186" s="17"/>
+      <c r="H186" s="17"/>
+      <c r="I186" s="17"/>
+      <c r="J186" s="17"/>
+      <c r="K186" s="17"/>
+      <c r="L186" s="17"/>
+      <c r="M186" s="17"/>
+      <c r="N186" s="17"/>
+      <c r="O186" s="17"/>
+      <c r="P186" s="17"/>
+      <c r="Q186" s="17"/>
+      <c r="R186" s="17"/>
+      <c r="S186" s="17"/>
+      <c r="T186" s="9"/>
+    </row>
+    <row r="187" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B187" s="8"/>
+      <c r="C187" s="17"/>
+      <c r="D187" s="17"/>
+      <c r="E187" s="17"/>
+      <c r="F187" s="17"/>
+      <c r="G187" s="17"/>
+      <c r="H187" s="17"/>
+      <c r="I187" s="17"/>
+      <c r="J187" s="17"/>
+      <c r="K187" s="17"/>
+      <c r="L187" s="17"/>
+      <c r="M187" s="17"/>
+      <c r="N187" s="17"/>
+      <c r="O187" s="17"/>
+      <c r="P187" s="17"/>
+      <c r="Q187" s="17"/>
+      <c r="R187" s="17"/>
+      <c r="S187" s="17"/>
+      <c r="T187" s="9"/>
+    </row>
+    <row r="188" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B188" s="8"/>
+      <c r="C188" s="17"/>
+      <c r="D188" s="17"/>
+      <c r="E188" s="17"/>
+      <c r="F188" s="17"/>
+      <c r="G188" s="17"/>
+      <c r="H188" s="17"/>
+      <c r="I188" s="17"/>
+      <c r="J188" s="17"/>
+      <c r="K188" s="17"/>
+      <c r="L188" s="17"/>
+      <c r="M188" s="17"/>
+      <c r="N188" s="17"/>
+      <c r="O188" s="17"/>
+      <c r="P188" s="17"/>
+      <c r="Q188" s="17"/>
+      <c r="R188" s="17"/>
+      <c r="S188" s="17"/>
+      <c r="T188" s="9"/>
+    </row>
+    <row r="189" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B189" s="8"/>
+      <c r="C189" s="17"/>
+      <c r="D189" s="17"/>
+      <c r="E189" s="17"/>
+      <c r="F189" s="17"/>
+      <c r="G189" s="17"/>
+      <c r="H189" s="17"/>
+      <c r="I189" s="17"/>
+      <c r="J189" s="17"/>
+      <c r="K189" s="17"/>
+      <c r="L189" s="17"/>
+      <c r="M189" s="17"/>
+      <c r="N189" s="17"/>
+      <c r="O189" s="17"/>
+      <c r="P189" s="17"/>
+      <c r="Q189" s="17"/>
+      <c r="R189" s="17"/>
+      <c r="S189" s="17"/>
+      <c r="T189" s="9"/>
+    </row>
+    <row r="190" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B190" s="8"/>
+      <c r="C190" s="17"/>
+      <c r="D190" s="17"/>
+      <c r="E190" s="17"/>
+      <c r="F190" s="17"/>
+      <c r="G190" s="17"/>
+      <c r="H190" s="17"/>
+      <c r="I190" s="17"/>
+      <c r="J190" s="17"/>
+      <c r="K190" s="17"/>
+      <c r="L190" s="17"/>
+      <c r="M190" s="17"/>
+      <c r="N190" s="17"/>
+      <c r="O190" s="17"/>
+      <c r="P190" s="17"/>
+      <c r="Q190" s="17"/>
+      <c r="R190" s="17"/>
+      <c r="S190" s="17"/>
+      <c r="T190" s="9"/>
+    </row>
+    <row r="191" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B191" s="8"/>
+      <c r="C191" s="17"/>
+      <c r="D191" s="17"/>
+      <c r="E191" s="17"/>
+      <c r="F191" s="17"/>
+      <c r="G191" s="17"/>
+      <c r="H191" s="17"/>
+      <c r="I191" s="17"/>
+      <c r="J191" s="17"/>
+      <c r="K191" s="17"/>
+      <c r="L191" s="17"/>
+      <c r="M191" s="17"/>
+      <c r="N191" s="17"/>
+      <c r="O191" s="17"/>
+      <c r="P191" s="17"/>
+      <c r="Q191" s="17"/>
+      <c r="R191" s="17"/>
+      <c r="S191" s="17"/>
+      <c r="T191" s="9"/>
+    </row>
+    <row r="192" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B192" s="8"/>
+      <c r="C192" s="17"/>
+      <c r="D192" s="17"/>
+      <c r="E192" s="17"/>
+      <c r="F192" s="17"/>
+      <c r="G192" s="17"/>
+      <c r="H192" s="17"/>
+      <c r="I192" s="17"/>
+      <c r="J192" s="17"/>
+      <c r="K192" s="17"/>
+      <c r="L192" s="17"/>
+      <c r="M192" s="17"/>
+      <c r="N192" s="17"/>
+      <c r="O192" s="17"/>
+      <c r="P192" s="17"/>
+      <c r="Q192" s="17"/>
+      <c r="R192" s="17"/>
+      <c r="S192" s="17"/>
+      <c r="T192" s="9"/>
+    </row>
+    <row r="193" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B193" s="8"/>
+      <c r="C193" s="17"/>
+      <c r="D193" s="17"/>
+      <c r="E193" s="17"/>
+      <c r="F193" s="17"/>
+      <c r="G193" s="17"/>
+      <c r="H193" s="17"/>
+      <c r="I193" s="17"/>
+      <c r="J193" s="17"/>
+      <c r="K193" s="17"/>
+      <c r="L193" s="17"/>
+      <c r="M193" s="17"/>
+      <c r="N193" s="17"/>
+      <c r="O193" s="17"/>
+      <c r="P193" s="17"/>
+      <c r="Q193" s="17"/>
+      <c r="R193" s="17"/>
+      <c r="S193" s="17"/>
+      <c r="T193" s="9"/>
+    </row>
+    <row r="194" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B194" s="8"/>
+      <c r="C194" s="17"/>
+      <c r="D194" s="17"/>
+      <c r="E194" s="17"/>
+      <c r="F194" s="17"/>
+      <c r="G194" s="17"/>
+      <c r="H194" s="17"/>
+      <c r="I194" s="17"/>
+      <c r="J194" s="17"/>
+      <c r="K194" s="17"/>
+      <c r="L194" s="17"/>
+      <c r="M194" s="17"/>
+      <c r="N194" s="17"/>
+      <c r="O194" s="17"/>
+      <c r="P194" s="17"/>
+      <c r="Q194" s="17"/>
+      <c r="R194" s="17"/>
+      <c r="S194" s="17"/>
+      <c r="T194" s="9"/>
+    </row>
+    <row r="195" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B195" s="8"/>
+      <c r="C195" s="17"/>
+      <c r="D195" s="17"/>
+      <c r="E195" s="17"/>
+      <c r="F195" s="17"/>
+      <c r="G195" s="17"/>
+      <c r="H195" s="17"/>
+      <c r="I195" s="17"/>
+      <c r="J195" s="17"/>
+      <c r="K195" s="17"/>
+      <c r="L195" s="17"/>
+      <c r="M195" s="17"/>
+      <c r="N195" s="17"/>
+      <c r="O195" s="17"/>
+      <c r="P195" s="17"/>
+      <c r="Q195" s="17"/>
+      <c r="R195" s="17"/>
+      <c r="S195" s="17"/>
+      <c r="T195" s="9"/>
+    </row>
+    <row r="196" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B196" s="8"/>
+      <c r="C196" s="17"/>
+      <c r="D196" s="17"/>
+      <c r="E196" s="17"/>
+      <c r="F196" s="17"/>
+      <c r="G196" s="17"/>
+      <c r="H196" s="17"/>
+      <c r="I196" s="17"/>
+      <c r="J196" s="17"/>
+      <c r="K196" s="17"/>
+      <c r="L196" s="17"/>
+      <c r="M196" s="17"/>
+      <c r="N196" s="17"/>
+      <c r="O196" s="17"/>
+      <c r="P196" s="17"/>
+      <c r="Q196" s="17"/>
+      <c r="R196" s="17"/>
+      <c r="S196" s="17"/>
+      <c r="T196" s="9"/>
+    </row>
+    <row r="197" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B197" s="8"/>
+      <c r="C197" s="17"/>
+      <c r="D197" s="17"/>
+      <c r="E197" s="17"/>
+      <c r="F197" s="17"/>
+      <c r="G197" s="17"/>
+      <c r="H197" s="17"/>
+      <c r="I197" s="17"/>
+      <c r="J197" s="17"/>
+      <c r="K197" s="17"/>
+      <c r="L197" s="17"/>
+      <c r="M197" s="17"/>
+      <c r="N197" s="17"/>
+      <c r="O197" s="17"/>
+      <c r="P197" s="17"/>
+      <c r="Q197" s="17"/>
+      <c r="R197" s="17"/>
+      <c r="S197" s="17"/>
+      <c r="T197" s="9"/>
+    </row>
+    <row r="198" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B198" s="8"/>
+      <c r="C198" s="17"/>
+      <c r="D198" s="17"/>
+      <c r="E198" s="17"/>
+      <c r="F198" s="17"/>
+      <c r="G198" s="17"/>
+      <c r="H198" s="17"/>
+      <c r="I198" s="17"/>
+      <c r="J198" s="17"/>
+      <c r="K198" s="17"/>
+      <c r="L198" s="17"/>
+      <c r="M198" s="17"/>
+      <c r="N198" s="17"/>
+      <c r="O198" s="17"/>
+      <c r="P198" s="17"/>
+      <c r="Q198" s="17"/>
+      <c r="R198" s="17"/>
+      <c r="S198" s="17"/>
+      <c r="T198" s="9"/>
+    </row>
+    <row r="199" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B199" s="8"/>
+      <c r="C199" s="17"/>
+      <c r="D199" s="17"/>
+      <c r="E199" s="17"/>
+      <c r="F199" s="17"/>
+      <c r="G199" s="17"/>
+      <c r="H199" s="17"/>
+      <c r="I199" s="17"/>
+      <c r="J199" s="17"/>
+      <c r="K199" s="17"/>
+      <c r="L199" s="17"/>
+      <c r="M199" s="17"/>
+      <c r="N199" s="17"/>
+      <c r="O199" s="17"/>
+      <c r="P199" s="17"/>
+      <c r="Q199" s="17"/>
+      <c r="R199" s="17"/>
+      <c r="S199" s="17"/>
+      <c r="T199" s="9"/>
+    </row>
+    <row r="200" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B200" s="8"/>
+      <c r="C200" s="17"/>
+      <c r="D200" s="17"/>
+      <c r="E200" s="17"/>
+      <c r="F200" s="17"/>
+      <c r="G200" s="17"/>
+      <c r="H200" s="17"/>
+      <c r="I200" s="17"/>
+      <c r="J200" s="17"/>
+      <c r="K200" s="17"/>
+      <c r="L200" s="17"/>
+      <c r="M200" s="17"/>
+      <c r="N200" s="17"/>
+      <c r="O200" s="17"/>
+      <c r="P200" s="17"/>
+      <c r="Q200" s="17"/>
+      <c r="R200" s="17"/>
+      <c r="S200" s="17"/>
+      <c r="T200" s="9"/>
+    </row>
+    <row r="201" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B201" s="8"/>
+      <c r="C201" s="17"/>
+      <c r="D201" s="17"/>
+      <c r="E201" s="17"/>
+      <c r="F201" s="17"/>
+      <c r="G201" s="17"/>
+      <c r="H201" s="17"/>
+      <c r="I201" s="17"/>
+      <c r="J201" s="17"/>
+      <c r="K201" s="17"/>
+      <c r="L201" s="17"/>
+      <c r="M201" s="17"/>
+      <c r="N201" s="17"/>
+      <c r="O201" s="17"/>
+      <c r="P201" s="17"/>
+      <c r="Q201" s="17"/>
+      <c r="R201" s="17"/>
+      <c r="S201" s="17"/>
+      <c r="T201" s="9"/>
+    </row>
+    <row r="202" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B202" s="8"/>
+      <c r="C202" s="17"/>
+      <c r="D202" s="17"/>
+      <c r="E202" s="17"/>
+      <c r="F202" s="17"/>
+      <c r="G202" s="17"/>
+      <c r="H202" s="17"/>
+      <c r="I202" s="17"/>
+      <c r="J202" s="17"/>
+      <c r="K202" s="17"/>
+      <c r="L202" s="17"/>
+      <c r="M202" s="17"/>
+      <c r="N202" s="17"/>
+      <c r="O202" s="17"/>
+      <c r="P202" s="17"/>
+      <c r="Q202" s="17"/>
+      <c r="R202" s="17"/>
+      <c r="S202" s="17"/>
+      <c r="T202" s="9"/>
+    </row>
+    <row r="203" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B203" s="8"/>
+      <c r="C203" s="17"/>
+      <c r="D203" s="17"/>
+      <c r="E203" s="17"/>
+      <c r="F203" s="17"/>
+      <c r="G203" s="17"/>
+      <c r="H203" s="17"/>
+      <c r="I203" s="17"/>
+      <c r="J203" s="17"/>
+      <c r="K203" s="17"/>
+      <c r="L203" s="17"/>
+      <c r="M203" s="17"/>
+      <c r="N203" s="17"/>
+      <c r="O203" s="17"/>
+      <c r="P203" s="17"/>
+      <c r="Q203" s="17"/>
+      <c r="R203" s="17"/>
+      <c r="S203" s="17"/>
+      <c r="T203" s="9"/>
+    </row>
+    <row r="204" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B204" s="8"/>
+      <c r="C204" s="17"/>
+      <c r="D204" s="17"/>
+      <c r="E204" s="17"/>
+      <c r="F204" s="17"/>
+      <c r="G204" s="17"/>
+      <c r="H204" s="17"/>
+      <c r="I204" s="17"/>
+      <c r="J204" s="17"/>
+      <c r="K204" s="17"/>
+      <c r="L204" s="17"/>
+      <c r="M204" s="17"/>
+      <c r="N204" s="17"/>
+      <c r="O204" s="17"/>
+      <c r="P204" s="17"/>
+      <c r="Q204" s="17"/>
+      <c r="R204" s="17"/>
+      <c r="S204" s="17"/>
+      <c r="T204" s="9"/>
+    </row>
+    <row r="205" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B205" s="8"/>
+      <c r="C205" s="17"/>
+      <c r="D205" s="17"/>
+      <c r="E205" s="17"/>
+      <c r="F205" s="17"/>
+      <c r="G205" s="17"/>
+      <c r="H205" s="17"/>
+      <c r="I205" s="17"/>
+      <c r="J205" s="17"/>
+      <c r="K205" s="17"/>
+      <c r="L205" s="17"/>
+      <c r="M205" s="17"/>
+      <c r="N205" s="17"/>
+      <c r="O205" s="17"/>
+      <c r="P205" s="17"/>
+      <c r="Q205" s="17"/>
+      <c r="R205" s="17"/>
+      <c r="S205" s="17"/>
+      <c r="T205" s="9"/>
+    </row>
+    <row r="206" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B206" s="8"/>
+      <c r="C206" s="17"/>
+      <c r="D206" s="17"/>
+      <c r="E206" s="17"/>
+      <c r="F206" s="17"/>
+      <c r="G206" s="17"/>
+      <c r="H206" s="17"/>
+      <c r="I206" s="17"/>
+      <c r="J206" s="17"/>
+      <c r="K206" s="17"/>
+      <c r="L206" s="17"/>
+      <c r="M206" s="17"/>
+      <c r="N206" s="17"/>
+      <c r="O206" s="17"/>
+      <c r="P206" s="17"/>
+      <c r="Q206" s="17"/>
+      <c r="R206" s="17"/>
+      <c r="S206" s="17"/>
+      <c r="T206" s="9"/>
+    </row>
+    <row r="207" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B207" s="8"/>
+      <c r="C207" s="17"/>
+      <c r="D207" s="17"/>
+      <c r="E207" s="17"/>
+      <c r="F207" s="17"/>
+      <c r="G207" s="17"/>
+      <c r="H207" s="17"/>
+      <c r="I207" s="17"/>
+      <c r="J207" s="17"/>
+      <c r="K207" s="17"/>
+      <c r="L207" s="17"/>
+      <c r="M207" s="17"/>
+      <c r="N207" s="17"/>
+      <c r="O207" s="17"/>
+      <c r="P207" s="17"/>
+      <c r="Q207" s="17"/>
+      <c r="R207" s="17"/>
+      <c r="S207" s="17"/>
+      <c r="T207" s="9"/>
+    </row>
+    <row r="208" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B208" s="8"/>
+      <c r="C208" s="17"/>
+      <c r="D208" s="17"/>
+      <c r="E208" s="17"/>
+      <c r="F208" s="17"/>
+      <c r="G208" s="17"/>
+      <c r="H208" s="17"/>
+      <c r="I208" s="17"/>
+      <c r="J208" s="17"/>
+      <c r="K208" s="17"/>
+      <c r="L208" s="17"/>
+      <c r="M208" s="17"/>
+      <c r="N208" s="17"/>
+      <c r="O208" s="17"/>
+      <c r="P208" s="17"/>
+      <c r="Q208" s="17"/>
+      <c r="R208" s="17"/>
+      <c r="S208" s="17"/>
+      <c r="T208" s="9"/>
+    </row>
+    <row r="209" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B209" s="8"/>
+      <c r="C209" s="17"/>
+      <c r="D209" s="17"/>
+      <c r="E209" s="17"/>
+      <c r="F209" s="17"/>
+      <c r="G209" s="17"/>
+      <c r="H209" s="17"/>
+      <c r="I209" s="17"/>
+      <c r="J209" s="17"/>
+      <c r="K209" s="17"/>
+      <c r="L209" s="17"/>
+      <c r="M209" s="17"/>
+      <c r="N209" s="17"/>
+      <c r="O209" s="17"/>
+      <c r="P209" s="17"/>
+      <c r="Q209" s="17"/>
+      <c r="R209" s="17"/>
+      <c r="S209" s="17"/>
+      <c r="T209" s="9"/>
+    </row>
+    <row r="210" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B210" s="8"/>
+      <c r="C210" s="17"/>
+      <c r="D210" s="17"/>
+      <c r="E210" s="17"/>
+      <c r="F210" s="17"/>
+      <c r="G210" s="17"/>
+      <c r="H210" s="17"/>
+      <c r="I210" s="17"/>
+      <c r="J210" s="17"/>
+      <c r="K210" s="17"/>
+      <c r="L210" s="17"/>
+      <c r="M210" s="17"/>
+      <c r="N210" s="17"/>
+      <c r="O210" s="17"/>
+      <c r="P210" s="17"/>
+      <c r="Q210" s="17"/>
+      <c r="R210" s="17"/>
+      <c r="S210" s="17"/>
+      <c r="T210" s="9"/>
+    </row>
+    <row r="211" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B211" s="8"/>
+      <c r="C211" s="17"/>
+      <c r="D211" s="17"/>
+      <c r="E211" s="17"/>
+      <c r="F211" s="17"/>
+      <c r="G211" s="17"/>
+      <c r="H211" s="17"/>
+      <c r="I211" s="17"/>
+      <c r="J211" s="17"/>
+      <c r="K211" s="17"/>
+      <c r="L211" s="17"/>
+      <c r="M211" s="17"/>
+      <c r="N211" s="17"/>
+      <c r="O211" s="17"/>
+      <c r="P211" s="17"/>
+      <c r="Q211" s="17"/>
+      <c r="R211" s="17"/>
+      <c r="S211" s="17"/>
+      <c r="T211" s="9"/>
+    </row>
+    <row r="212" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B212" s="8"/>
+      <c r="C212" s="17"/>
+      <c r="D212" s="17"/>
+      <c r="E212" s="17"/>
+      <c r="F212" s="17"/>
+      <c r="G212" s="17"/>
+      <c r="H212" s="17"/>
+      <c r="I212" s="17"/>
+      <c r="J212" s="17"/>
+      <c r="K212" s="17"/>
+      <c r="L212" s="17"/>
+      <c r="M212" s="17"/>
+      <c r="N212" s="17"/>
+      <c r="O212" s="17"/>
+      <c r="P212" s="17"/>
+      <c r="Q212" s="17"/>
+      <c r="R212" s="17"/>
+      <c r="S212" s="17"/>
+      <c r="T212" s="9"/>
+    </row>
+    <row r="213" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B213" s="8"/>
+      <c r="C213" s="17"/>
+      <c r="D213" s="17"/>
+      <c r="E213" s="17"/>
+      <c r="F213" s="17"/>
+      <c r="G213" s="17"/>
+      <c r="H213" s="17"/>
+      <c r="I213" s="17"/>
+      <c r="J213" s="17"/>
+      <c r="K213" s="17"/>
+      <c r="L213" s="17"/>
+      <c r="M213" s="17"/>
+      <c r="N213" s="17"/>
+      <c r="O213" s="17"/>
+      <c r="P213" s="17"/>
+      <c r="Q213" s="17"/>
+      <c r="R213" s="17"/>
+      <c r="S213" s="17"/>
+      <c r="T213" s="9"/>
+    </row>
+    <row r="214" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B214" s="8"/>
+      <c r="C214" s="17"/>
+      <c r="D214" s="17"/>
+      <c r="E214" s="17"/>
+      <c r="F214" s="17"/>
+      <c r="G214" s="17"/>
+      <c r="H214" s="17"/>
+      <c r="I214" s="17"/>
+      <c r="J214" s="17"/>
+      <c r="K214" s="17"/>
+      <c r="L214" s="17"/>
+      <c r="M214" s="17"/>
+      <c r="N214" s="17"/>
+      <c r="O214" s="17"/>
+      <c r="P214" s="17"/>
+      <c r="Q214" s="17"/>
+      <c r="R214" s="17"/>
+      <c r="S214" s="17"/>
+      <c r="T214" s="9"/>
+    </row>
+    <row r="215" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B215" s="8"/>
+      <c r="C215" s="17"/>
+      <c r="D215" s="17"/>
+      <c r="E215" s="17"/>
+      <c r="F215" s="17"/>
+      <c r="G215" s="17"/>
+      <c r="H215" s="17"/>
+      <c r="I215" s="17"/>
+      <c r="J215" s="17"/>
+      <c r="K215" s="17"/>
+      <c r="L215" s="17"/>
+      <c r="M215" s="17"/>
+      <c r="N215" s="17"/>
+      <c r="O215" s="17"/>
+      <c r="P215" s="17"/>
+      <c r="Q215" s="17"/>
+      <c r="R215" s="17"/>
+      <c r="S215" s="17"/>
+      <c r="T215" s="9"/>
+    </row>
+    <row r="216" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B216" s="8"/>
+      <c r="C216" s="17"/>
+      <c r="D216" s="17"/>
+      <c r="E216" s="17"/>
+      <c r="F216" s="17"/>
+      <c r="G216" s="17"/>
+      <c r="H216" s="17"/>
+      <c r="I216" s="17"/>
+      <c r="J216" s="17"/>
+      <c r="K216" s="17"/>
+      <c r="L216" s="17"/>
+      <c r="M216" s="17"/>
+      <c r="N216" s="17"/>
+      <c r="O216" s="17"/>
+      <c r="P216" s="17"/>
+      <c r="Q216" s="17"/>
+      <c r="R216" s="17"/>
+      <c r="S216" s="17"/>
+      <c r="T216" s="9"/>
+    </row>
+    <row r="217" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B217" s="8"/>
+      <c r="C217" s="17"/>
+      <c r="D217" s="17"/>
+      <c r="E217" s="17"/>
+      <c r="F217" s="17"/>
+      <c r="G217" s="17"/>
+      <c r="H217" s="17"/>
+      <c r="I217" s="17"/>
+      <c r="J217" s="17"/>
+      <c r="K217" s="17"/>
+      <c r="L217" s="17"/>
+      <c r="M217" s="17"/>
+      <c r="N217" s="17"/>
+      <c r="O217" s="17"/>
+      <c r="P217" s="17"/>
+      <c r="Q217" s="17"/>
+      <c r="R217" s="17"/>
+      <c r="S217" s="17"/>
+      <c r="T217" s="9"/>
+    </row>
+    <row r="218" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B218" s="8"/>
+      <c r="C218" s="17"/>
+      <c r="D218" s="17"/>
+      <c r="E218" s="17"/>
+      <c r="F218" s="17"/>
+      <c r="G218" s="17"/>
+      <c r="H218" s="17"/>
+      <c r="I218" s="17"/>
+      <c r="J218" s="17"/>
+      <c r="K218" s="17"/>
+      <c r="L218" s="17"/>
+      <c r="M218" s="17"/>
+      <c r="N218" s="17"/>
+      <c r="O218" s="17"/>
+      <c r="P218" s="17"/>
+      <c r="Q218" s="17"/>
+      <c r="R218" s="17"/>
+      <c r="S218" s="17"/>
+      <c r="T218" s="9"/>
+    </row>
+    <row r="219" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B219" s="8"/>
+      <c r="C219" s="17"/>
+      <c r="D219" s="17"/>
+      <c r="E219" s="17"/>
+      <c r="F219" s="17"/>
+      <c r="G219" s="17"/>
+      <c r="H219" s="17"/>
+      <c r="I219" s="17"/>
+      <c r="J219" s="17"/>
+      <c r="K219" s="17"/>
+      <c r="L219" s="17"/>
+      <c r="M219" s="17"/>
+      <c r="N219" s="17"/>
+      <c r="O219" s="17"/>
+      <c r="P219" s="17"/>
+      <c r="Q219" s="17"/>
+      <c r="R219" s="17"/>
+      <c r="S219" s="17"/>
+      <c r="T219" s="9"/>
+    </row>
+    <row r="220" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B220" s="8"/>
+      <c r="C220" s="17"/>
+      <c r="D220" s="17"/>
+      <c r="E220" s="17"/>
+      <c r="F220" s="17"/>
+      <c r="G220" s="17"/>
+      <c r="H220" s="17"/>
+      <c r="I220" s="17"/>
+      <c r="J220" s="17"/>
+      <c r="K220" s="17"/>
+      <c r="L220" s="17"/>
+      <c r="M220" s="17"/>
+      <c r="N220" s="17"/>
+      <c r="O220" s="17"/>
+      <c r="P220" s="17"/>
+      <c r="Q220" s="17"/>
+      <c r="R220" s="17"/>
+      <c r="S220" s="17"/>
+      <c r="T220" s="9"/>
+    </row>
+    <row r="221" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B221" s="8"/>
+      <c r="C221" s="17"/>
+      <c r="D221" s="17"/>
+      <c r="E221" s="17"/>
+      <c r="F221" s="17"/>
+      <c r="G221" s="17"/>
+      <c r="H221" s="17"/>
+      <c r="I221" s="17"/>
+      <c r="J221" s="17"/>
+      <c r="K221" s="17"/>
+      <c r="L221" s="17"/>
+      <c r="M221" s="17"/>
+      <c r="N221" s="17"/>
+      <c r="O221" s="17"/>
+      <c r="P221" s="17"/>
+      <c r="Q221" s="17"/>
+      <c r="R221" s="17"/>
+      <c r="S221" s="17"/>
+      <c r="T221" s="9"/>
+    </row>
+    <row r="222" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B222" s="8"/>
+      <c r="C222" s="17"/>
+      <c r="D222" s="17"/>
+      <c r="E222" s="17"/>
+      <c r="F222" s="17"/>
+      <c r="G222" s="17"/>
+      <c r="H222" s="17"/>
+      <c r="I222" s="17"/>
+      <c r="J222" s="17"/>
+      <c r="K222" s="17"/>
+      <c r="L222" s="17"/>
+      <c r="M222" s="17"/>
+      <c r="N222" s="17"/>
+      <c r="O222" s="17"/>
+      <c r="P222" s="17"/>
+      <c r="Q222" s="17"/>
+      <c r="R222" s="17"/>
+      <c r="S222" s="17"/>
+      <c r="T222" s="9"/>
+    </row>
+    <row r="223" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B223" s="8"/>
+      <c r="C223" s="17"/>
+      <c r="D223" s="17"/>
+      <c r="E223" s="17"/>
+      <c r="F223" s="17"/>
+      <c r="G223" s="17"/>
+      <c r="H223" s="17"/>
+      <c r="I223" s="17"/>
+      <c r="J223" s="17"/>
+      <c r="K223" s="17"/>
+      <c r="L223" s="17"/>
+      <c r="M223" s="17"/>
+      <c r="N223" s="17"/>
+      <c r="O223" s="17"/>
+      <c r="P223" s="17"/>
+      <c r="Q223" s="17"/>
+      <c r="R223" s="17"/>
+      <c r="S223" s="17"/>
+      <c r="T223" s="9"/>
+    </row>
+    <row r="224" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B224" s="8"/>
+      <c r="C224" s="17"/>
+      <c r="D224" s="17"/>
+      <c r="E224" s="17"/>
+      <c r="F224" s="17"/>
+      <c r="G224" s="17"/>
+      <c r="H224" s="17"/>
+      <c r="I224" s="17"/>
+      <c r="J224" s="17"/>
+      <c r="K224" s="17"/>
+      <c r="L224" s="17"/>
+      <c r="M224" s="17"/>
+      <c r="N224" s="17"/>
+      <c r="O224" s="17"/>
+      <c r="P224" s="17"/>
+      <c r="Q224" s="17"/>
+      <c r="R224" s="17"/>
+      <c r="S224" s="17"/>
+      <c r="T224" s="9"/>
+    </row>
+    <row r="225" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B225" s="8"/>
+      <c r="C225" s="17"/>
+      <c r="D225" s="17"/>
+      <c r="E225" s="17"/>
+      <c r="F225" s="17"/>
+      <c r="G225" s="17"/>
+      <c r="H225" s="17"/>
+      <c r="I225" s="17"/>
+      <c r="J225" s="17"/>
+      <c r="K225" s="17"/>
+      <c r="L225" s="17"/>
+      <c r="M225" s="17"/>
+      <c r="N225" s="17"/>
+      <c r="O225" s="17"/>
+      <c r="P225" s="17"/>
+      <c r="Q225" s="17"/>
+      <c r="R225" s="17"/>
+      <c r="S225" s="17"/>
+      <c r="T225" s="9"/>
+    </row>
+    <row r="226" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B226" s="10"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="5"/>
+      <c r="E226" s="5"/>
+      <c r="F226" s="5"/>
+      <c r="G226" s="5"/>
+      <c r="H226" s="5"/>
+      <c r="I226" s="5"/>
+      <c r="J226" s="5"/>
+      <c r="K226" s="5"/>
+      <c r="L226" s="5"/>
+      <c r="M226" s="5"/>
+      <c r="N226" s="5"/>
+      <c r="O226" s="5"/>
+      <c r="P226" s="5"/>
+      <c r="Q226" s="5"/>
+      <c r="R226" s="5"/>
+      <c r="S226" s="5"/>
+      <c r="T226" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>